<commit_message>
select cell fix v1
</commit_message>
<xml_diff>
--- a/ExcelTests/ExcelTests/bin/Debug/TestFile1.xlsx
+++ b/ExcelTests/ExcelTests/bin/Debug/TestFile1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Ranorex Tests\Excel Tests\ExcelTests\ExcelTests\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FF6EEECB-30BD-46FA-99B7-E0CD4C3C8DF8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D799737-CC8B-4AD3-AC50-021BF623C085}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9915" xr2:uid="{4E79AE58-C853-47CF-8FBF-1D1B86DEC374}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9915" xr2:uid="{F32D55C7-17EE-4D6D-95D6-35DE63398838}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,14 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>ABC</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -370,16 +378,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6319C7F8-E479-4C46-85DF-19D1AED2CC77}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EBCC765-A5EF-4F9C-80D5-E5D74098492A}">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>10</v>
+      <c r="A1" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -403,9 +413,9 @@
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <f>(A1+A2)*A3+A4-A5</f>
-        <v>114</v>
+      <c r="A6" t="e">
+        <f>(A1+A2)*A3+A4+A5</f>
+        <v>#VALUE!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>